<commit_message>
#71 moved agreement checkboxes
</commit_message>
<xml_diff>
--- a/documents/side files/market-comparison.xlsx
+++ b/documents/side files/market-comparison.xlsx
@@ -162,7 +162,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -174,6 +174,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -187,7 +190,47 @@
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="18">
+  <dxfs count="22">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -668,7 +711,7 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -683,10 +726,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5"/>
+      <c r="B1" s="6"/>
       <c r="C1" s="3" t="s">
         <v>14</v>
       </c>
@@ -710,7 +753,7 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="4" t="s">
@@ -739,7 +782,7 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="6"/>
+      <c r="A3" s="7"/>
       <c r="B3" s="4" t="s">
         <v>24</v>
       </c>
@@ -766,7 +809,7 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="6"/>
+      <c r="A4" s="7"/>
       <c r="B4" s="4" t="s">
         <v>2</v>
       </c>
@@ -793,7 +836,7 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="6"/>
+      <c r="A5" s="7"/>
       <c r="B5" s="4" t="s">
         <v>3</v>
       </c>
@@ -820,7 +863,7 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="6"/>
+      <c r="A6" s="7"/>
       <c r="B6" s="4" t="s">
         <v>23</v>
       </c>
@@ -847,7 +890,7 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="8" t="s">
         <v>8</v>
       </c>
       <c r="B7" s="4" t="s">
@@ -871,12 +914,12 @@
       <c r="H7" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="I7" s="3" t="s">
-        <v>27</v>
+      <c r="I7" s="5" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="7"/>
+      <c r="A8" s="8"/>
       <c r="B8" s="4" t="s">
         <v>6</v>
       </c>
@@ -903,7 +946,7 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="7"/>
+      <c r="A9" s="8"/>
       <c r="B9" s="4" t="s">
         <v>7</v>
       </c>
@@ -930,10 +973,10 @@
       </c>
     </row>
     <row r="10" spans="1:9" s="1" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="7"/>
+      <c r="B10" s="8"/>
       <c r="C10" s="2" t="s">
         <v>29</v>
       </c>
@@ -957,7 +1000,7 @@
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="7" t="s">
         <v>13</v>
       </c>
       <c r="B11" s="4" t="s">
@@ -986,7 +1029,7 @@
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="6"/>
+      <c r="A12" s="7"/>
       <c r="B12" s="4" t="s">
         <v>11</v>
       </c>
@@ -1013,7 +1056,7 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="6"/>
+      <c r="A13" s="7"/>
       <c r="B13" s="4" t="s">
         <v>12</v>
       </c>
@@ -1048,27 +1091,27 @@
     <mergeCell ref="A11:A13"/>
   </mergeCells>
   <conditionalFormatting sqref="C10:I10">
-    <cfRule type="containsText" dxfId="17" priority="17" operator="containsText" text="без дополнительной комиссии">
+    <cfRule type="containsText" dxfId="21" priority="17" operator="containsText" text="без дополнительной комиссии">
       <formula>NOT(ISERROR(SEARCH("без дополнительной комиссии",C10)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="18" operator="containsText" text="Ежемесячная подписка">
+    <cfRule type="containsText" dxfId="20" priority="18" operator="containsText" text="Ежемесячная подписка">
       <formula>NOT(ISERROR(SEARCH("Ежемесячная подписка",C10)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="15" priority="19" operator="containsText" text="Пропорционально билету">
+    <cfRule type="containsText" dxfId="19" priority="19" operator="containsText" text="Пропорционально билету">
       <formula>NOT(ISERROR(SEARCH("Пропорционально билету",C10)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:I9">
-    <cfRule type="containsText" dxfId="14" priority="10" operator="containsText" text="не реализовано">
+    <cfRule type="containsText" dxfId="18" priority="10" operator="containsText" text="не реализовано">
       <formula>NOT(ISERROR(SEARCH("не реализовано",C2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="11" operator="containsText" text="требует разработки">
+    <cfRule type="containsText" dxfId="17" priority="11" operator="containsText" text="требует разработки">
       <formula>NOT(ISERROR(SEARCH("требует разработки",C2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="13" operator="containsText" text="затратно">
+    <cfRule type="containsText" dxfId="16" priority="13" operator="containsText" text="затратно">
       <formula>NOT(ISERROR(SEARCH("затратно",C2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="11" priority="14" operator="containsText" text="доступно">
+    <cfRule type="containsText" dxfId="15" priority="14" operator="containsText" text="доступно">
       <formula>NOT(ISERROR(SEARCH("доступно",C2)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1138,32 +1181,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="7" t="s">
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7" t="s">
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="K1" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="6"/>
+      <c r="A2" s="7"/>
       <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
@@ -1188,7 +1231,7 @@
       <c r="I2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="7"/>
+      <c r="J2" s="8"/>
       <c r="K2" s="3" t="s">
         <v>10</v>
       </c>
@@ -1495,27 +1538,27 @@
     <mergeCell ref="B1:F1"/>
   </mergeCells>
   <conditionalFormatting sqref="J3:J9">
-    <cfRule type="containsText" dxfId="8" priority="7" operator="containsText" text="без дополнительной комиссии">
+    <cfRule type="containsText" dxfId="12" priority="7" operator="containsText" text="без дополнительной комиссии">
       <formula>NOT(ISERROR(SEARCH("без дополнительной комиссии",J3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="Ежемесячная подписка">
+    <cfRule type="containsText" dxfId="11" priority="8" operator="containsText" text="Ежемесячная подписка">
       <formula>NOT(ISERROR(SEARCH("Ежемесячная подписка",J3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="9" operator="containsText" text="Пропорционально билету">
+    <cfRule type="containsText" dxfId="10" priority="9" operator="containsText" text="Пропорционально билету">
       <formula>NOT(ISERROR(SEARCH("Пропорционально билету",J3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:I9">
-    <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="не реализовано">
+    <cfRule type="containsText" dxfId="9" priority="1" operator="containsText" text="не реализовано">
       <formula>NOT(ISERROR(SEARCH("не реализовано",B3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="требует разработки">
+    <cfRule type="containsText" dxfId="8" priority="2" operator="containsText" text="требует разработки">
       <formula>NOT(ISERROR(SEARCH("требует разработки",B3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="затратно">
+    <cfRule type="containsText" dxfId="7" priority="3" operator="containsText" text="затратно">
       <formula>NOT(ISERROR(SEARCH("затратно",B3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="доступно">
+    <cfRule type="containsText" dxfId="6" priority="4" operator="containsText" text="доступно">
       <formula>NOT(ISERROR(SEARCH("доступно",B3)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>